<commit_message>
Update of Excel Modules Files
</commit_message>
<xml_diff>
--- a/resources/G3EI1/modules.xlsx
+++ b/resources/G3EI1/modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\G3EI1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EFD883-26BD-4359-B099-F9BCBC66A5EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C73BDCB-7BCE-4C1C-A88A-4BA9F01F9D36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{940AF663-DFD1-40C0-8D22-F4D1A033E9DA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Code</t>
   </si>
@@ -42,9 +42,6 @@
     <t>ElementName2</t>
   </si>
   <si>
-    <t>ElementName3</t>
-  </si>
-  <si>
     <t>G3EI111</t>
   </si>
   <si>
@@ -79,6 +76,135 @@
   </si>
   <si>
     <t>G3EI125</t>
+  </si>
+  <si>
+    <t>pede. Suspendisse dui.</t>
+  </si>
+  <si>
+    <t>EL Haddad</t>
+  </si>
+  <si>
+    <t>Nullam feugiat placerat</t>
+  </si>
+  <si>
+    <t>varius et, euismod</t>
+  </si>
+  <si>
+    <t>a nunc. In</t>
+  </si>
+  <si>
+    <t>Badir</t>
+  </si>
+  <si>
+    <t>sodales nisi magna</t>
+  </si>
+  <si>
+    <t>elementum sem, vitae</t>
+  </si>
+  <si>
+    <t>amet metus. Aliquam</t>
+  </si>
+  <si>
+    <t>Ezzine</t>
+  </si>
+  <si>
+    <t>Cras vulputate velit</t>
+  </si>
+  <si>
+    <t>scelerisque neque sed</t>
+  </si>
+  <si>
+    <t>quam vel sapien</t>
+  </si>
+  <si>
+    <t>El Alami Hassoun</t>
+  </si>
+  <si>
+    <t>Nunc mauris elit,</t>
+  </si>
+  <si>
+    <t>libero et tristique</t>
+  </si>
+  <si>
+    <t>feugiat nec, diam.</t>
+  </si>
+  <si>
+    <t>Lazaar</t>
+  </si>
+  <si>
+    <t>pellentesque. Sed dictum.</t>
+  </si>
+  <si>
+    <t>ridiculus mus. Proin</t>
+  </si>
+  <si>
+    <t>nonummy. Fusce fermentum</t>
+  </si>
+  <si>
+    <t>El Haddad</t>
+  </si>
+  <si>
+    <t>neque pellentesque massa</t>
+  </si>
+  <si>
+    <t>Mauris eu turpis.</t>
+  </si>
+  <si>
+    <t>a, arcu. Sed</t>
+  </si>
+  <si>
+    <t>sit amet risus.</t>
+  </si>
+  <si>
+    <t>Nulla facilisi. Sed</t>
+  </si>
+  <si>
+    <t>Suspendisse eleifend. Cras</t>
+  </si>
+  <si>
+    <t>velit dui, semper</t>
+  </si>
+  <si>
+    <t>ligula elit, pretium</t>
+  </si>
+  <si>
+    <t>ante. Nunc mauris</t>
+  </si>
+  <si>
+    <t>tortor at risus.</t>
+  </si>
+  <si>
+    <t>felis. Donec tempor,</t>
+  </si>
+  <si>
+    <t>lobortis quam a</t>
+  </si>
+  <si>
+    <t>euismod est arcu</t>
+  </si>
+  <si>
+    <t>ligula eu enim.</t>
+  </si>
+  <si>
+    <t>rhoncus. Nullam velit</t>
+  </si>
+  <si>
+    <t>Ben Achrab</t>
+  </si>
+  <si>
+    <t>ut dolor dapibus</t>
+  </si>
+  <si>
+    <t>commodo tincidunt nibh.</t>
+  </si>
+  <si>
+    <t>Donec tincidunt. Donec</t>
+  </si>
+  <si>
+    <t>ornare tortor at</t>
+  </si>
+  <si>
+    <t>ac, feugiat non,</t>
   </si>
 </sst>
 </file>
@@ -430,21 +556,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A3A4ED-895E-481A-9310-6D535019DF80}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,68 +588,209 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>